<commit_message>
fixed final graph before bed, gnite
</commit_message>
<xml_diff>
--- a/experiments/compression/results xl.xlsx
+++ b/experiments/compression/results xl.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="low bitrate zoom" sheetId="3" r:id="rId1"/>
     <sheet name="main" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="ChartX" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -370,11 +371,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="436608736"/>
-        <c:axId val="436611088"/>
+        <c:axId val="322625936"/>
+        <c:axId val="322629072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="436608736"/>
+        <c:axId val="322625936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -422,7 +423,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -489,12 +489,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436611088"/>
+        <c:crossAx val="322629072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="436611088"/>
+        <c:axId val="322629072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="82"/>
@@ -542,7 +542,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -609,7 +608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436608736"/>
+        <c:crossAx val="322625936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -623,7 +622,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -929,11 +927,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="237041584"/>
-        <c:axId val="237038448"/>
+        <c:axId val="322629464"/>
+        <c:axId val="322630248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="237041584"/>
+        <c:axId val="322629464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220000"/>
@@ -1048,12 +1046,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237038448"/>
+        <c:crossAx val="322630248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237038448"/>
+        <c:axId val="322630248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -1168,7 +1166,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237041584"/>
+        <c:crossAx val="322629464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1279,6 +1277,503 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="50800">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184465</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>201209</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>201505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>78.331100000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.691000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101.208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103.76900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="50800">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21393</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>297585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>305649</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>315009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>78.331100000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.1845</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.326700000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103.76900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="360226168"/>
+        <c:axId val="360217152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="360226168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="220000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="4000"/>
+                  <a:t>Bits</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="360217152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="360217152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="110"/>
+          <c:min val="77"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="4000"/>
+                  <a:t>PSNR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="360226168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.45699722473215437"/>
+          <c:y val="6.4853556485355651E-2"/>
+          <c:w val="0.27999462157394261"/>
+          <c:h val="0.2099095641287517"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
@@ -1353,84 +1848,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ILOT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$3:$E$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>11409</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41489</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>137745</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$3:$F$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>79.029799999999994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>79.890100000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>81.742599999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$A$1</c:f>
@@ -1524,11 +1943,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="195138024"/>
-        <c:axId val="195139200"/>
+        <c:axId val="322631816"/>
+        <c:axId val="322624368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="195138024"/>
+        <c:axId val="322631816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220000"/>
@@ -1643,12 +2062,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195139200"/>
+        <c:crossAx val="322624368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="195139200"/>
+        <c:axId val="322624368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -1763,7 +2182,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195138024"/>
+        <c:crossAx val="322631816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1844,7 +2263,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2124,11 +2543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="237032568"/>
-        <c:axId val="237032960"/>
+        <c:axId val="324667896"/>
+        <c:axId val="324663976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="237032568"/>
+        <c:axId val="324667896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000"/>
@@ -2243,12 +2662,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237032960"/>
+        <c:crossAx val="324663976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237032960"/>
+        <c:axId val="324663976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="82"/>
@@ -2363,7 +2782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237032568"/>
+        <c:crossAx val="324667896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2604,6 +3023,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4153,6 +4612,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4680,6 +5655,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="75" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -4746,18 +5732,45 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5076,8 +6089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>